<commit_message>
Atualização PN e LE
Atualização PN e LE
</commit_message>
<xml_diff>
--- a/ModelagemDosProcessosDeNegocio/Lista de eventos - Agendar Consulta.xlsx
+++ b/ModelagemDosProcessosDeNegocio/Lista de eventos - Agendar Consulta.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1600192\Downloads\Takai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FIT\TCC.github.io\ModelagemDosProcessosDeNegocio\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -130,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
   <si>
     <t>Externo</t>
   </si>
@@ -184,6 +184,72 @@
   </si>
   <si>
     <t>Paciente solicita agendamento da consulta.</t>
+  </si>
+  <si>
+    <t>Receber
+Pagamento
+Empresa</t>
+  </si>
+  <si>
+    <t>Psicóloga finaliza a consulta</t>
+  </si>
+  <si>
+    <t>Psicóloga registra a cobrança do serviço em pastas no seu computador pessoal</t>
+  </si>
+  <si>
+    <t>x(1)</t>
+  </si>
+  <si>
+    <t>Psicóloga consolida cobrança de serviço</t>
+  </si>
+  <si>
+    <t>x(2)</t>
+  </si>
+  <si>
+    <t>Psicóloga envia consolidado de cobrança para empresa.</t>
+  </si>
+  <si>
+    <t>x(3)</t>
+  </si>
+  <si>
+    <t>Empresa efetua o pagamento</t>
+  </si>
+  <si>
+    <t>x(4)</t>
+  </si>
+  <si>
+    <t>FA</t>
+  </si>
+  <si>
+    <t>Empresa não efetua o pagamento</t>
+  </si>
+  <si>
+    <t>Receber
+Pagamento
+Particular</t>
+  </si>
+  <si>
+    <t>Informa o valor para o paciente</t>
+  </si>
+  <si>
+    <t>Paciente efetua o pagamento</t>
+  </si>
+  <si>
+    <t>Paciente não efetua o pagamento</t>
+  </si>
+  <si>
+    <t>Receber
+Pagamento
+Palestra</t>
+  </si>
+  <si>
+    <t>Psicóloga finaliza a palestra</t>
+  </si>
+  <si>
+    <t>Cliente efetua o pagamento</t>
+  </si>
+  <si>
+    <t>Cliente não efetua o pagamento</t>
   </si>
 </sst>
 </file>
@@ -259,7 +325,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -501,11 +567,81 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -543,9 +679,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -587,6 +720,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -868,15 +1028,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
     <col min="2" max="3" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" customWidth="1"/>
@@ -889,25 +1049,25 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="25"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="20" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="20" t="s">
+      <c r="F1" s="21"/>
+      <c r="G1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="21"/>
-      <c r="I1" s="22"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="21"/>
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="24"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="11" t="s">
         <v>3</v>
       </c>
@@ -934,10 +1094,10 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="12">
@@ -956,9 +1116,9 @@
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="13">
+      <c r="A4" s="14"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="12">
         <v>2</v>
       </c>
       <c r="D4" s="10" t="s">
@@ -974,9 +1134,9 @@
       <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="13">
+      <c r="A5" s="14"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="12">
         <v>3</v>
       </c>
       <c r="D5" s="10" t="s">
@@ -992,9 +1152,9 @@
       <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="13">
+      <c r="A6" s="15"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="12">
         <v>4</v>
       </c>
       <c r="D6" s="10" t="s">
@@ -1009,8 +1169,285 @@
       <c r="I6" s="7"/>
       <c r="J6" s="8"/>
     </row>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="12">
+        <v>5</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="27"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="12">
+        <v>6</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="27"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="12">
+        <v>7</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="27"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="12">
+        <v>8</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="27"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="12">
+        <v>9</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27"/>
+      <c r="B12" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="12">
+        <v>10</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="12">
+        <v>11</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="31"/>
+    </row>
+    <row r="14" spans="1:10" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="32"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="12">
+        <v>12</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="31"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="32"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="12">
+        <v>13</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="31"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="32"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="12">
+        <v>14</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="31"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="35"/>
+      <c r="B17" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="12">
+        <v>15</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="31"/>
+    </row>
+    <row r="18" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="12">
+        <v>16</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="7"/>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="32"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="12">
+        <v>17</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="6"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="35"/>
+      <c r="B20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="12">
+        <v>18</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="12">
+    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B19"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="G1:I1"/>

</xml_diff>